<commit_message>
Add ranking attributes and score to SPFH
</commit_message>
<xml_diff>
--- a/backend/app/sp500.xlsx
+++ b/backend/app/sp500.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WaThone\Documents\GitHub\AWSome\backend\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB67E3B-B9E2-43CE-ADE9-81296C1D5C68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7747468-F8F8-47A3-ACB8-953F1940703E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="18159" windowHeight="9715" xr2:uid="{5E18AD6D-D578-4283-9BA2-3786E51CE4A2}"/>
   </bookViews>
@@ -18,6 +18,7 @@
   <definedNames>
     <definedName name="Company_Names">Sheet1!$A$3:$A$507</definedName>
     <definedName name="Exchange_Ticker">Sheet1!#REF!</definedName>
+    <definedName name="Ticker">Sheet1!$B$2:$B$501</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="9.9999999999994451E-4"/>
   <extLst>
@@ -1734,9 +1735,6 @@
     <t>CPRT</t>
   </si>
   <si>
-    <t>BF.B</t>
-  </si>
-  <si>
     <t>KMB</t>
   </si>
   <si>
@@ -2322,9 +2320,6 @@
     <t>XYL</t>
   </si>
   <si>
-    <t>CMCS.A</t>
-  </si>
-  <si>
     <t>WEC</t>
   </si>
   <si>
@@ -2421,9 +2416,6 @@
     <t>CMI</t>
   </si>
   <si>
-    <t>DISC.K</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -2535,9 +2527,6 @@
     <t>CNP</t>
   </si>
   <si>
-    <t>BRK.B</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -3043,6 +3032,18 @@
   </si>
   <si>
     <t>NCLH</t>
+  </si>
+  <si>
+    <t>BFB</t>
+  </si>
+  <si>
+    <t>CMCSA</t>
+  </si>
+  <si>
+    <t>DISCK</t>
+  </si>
+  <si>
+    <t>BRKB</t>
   </si>
 </sst>
 </file>
@@ -3426,7 +3427,7 @@
   <dimension ref="A1:B507"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B500" sqref="B1:B500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.1" x14ac:dyDescent="0.35"/>
@@ -3952,7 +3953,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>565</v>
+        <v>998</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -3960,7 +3961,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
@@ -3968,7 +3969,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
@@ -3976,7 +3977,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -3984,7 +3985,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
@@ -3992,7 +3993,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
@@ -4000,7 +4001,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -4008,7 +4009,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -4016,7 +4017,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -4024,7 +4025,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -4032,7 +4033,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -4040,7 +4041,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -4048,7 +4049,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
@@ -4056,7 +4057,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -4064,7 +4065,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
@@ -4072,7 +4073,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
@@ -4080,7 +4081,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -4088,7 +4089,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -4096,7 +4097,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -4104,7 +4105,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -4112,7 +4113,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -4120,7 +4121,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -4128,7 +4129,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -4136,7 +4137,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -4144,7 +4145,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -4152,7 +4153,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -4160,7 +4161,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
@@ -4168,7 +4169,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -4176,7 +4177,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
@@ -4184,7 +4185,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
@@ -4192,7 +4193,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -4200,7 +4201,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
@@ -4208,7 +4209,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
@@ -4216,7 +4217,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -4224,7 +4225,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -4232,7 +4233,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
@@ -4240,7 +4241,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
@@ -4248,7 +4249,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -4256,7 +4257,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
@@ -4264,7 +4265,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
@@ -4272,7 +4273,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
@@ -4280,7 +4281,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
@@ -4288,7 +4289,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
@@ -4296,7 +4297,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -4304,7 +4305,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
@@ -4312,7 +4313,7 @@
         <v>108</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -4320,7 +4321,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -4328,7 +4329,7 @@
         <v>110</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -4336,7 +4337,7 @@
         <v>111</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
@@ -4344,7 +4345,7 @@
         <v>112</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -4352,7 +4353,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -4360,7 +4361,7 @@
         <v>114</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -4368,7 +4369,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -4376,7 +4377,7 @@
         <v>116</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
@@ -4384,7 +4385,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -4392,7 +4393,7 @@
         <v>118</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -4400,7 +4401,7 @@
         <v>119</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
@@ -4408,7 +4409,7 @@
         <v>120</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -4416,7 +4417,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -4424,7 +4425,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -4432,7 +4433,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
@@ -4440,7 +4441,7 @@
         <v>124</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
@@ -4448,7 +4449,7 @@
         <v>125</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -4456,7 +4457,7 @@
         <v>126</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
@@ -4464,7 +4465,7 @@
         <v>127</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
@@ -4472,7 +4473,7 @@
         <v>128</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
@@ -4480,7 +4481,7 @@
         <v>129</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
@@ -4488,7 +4489,7 @@
         <v>130</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
@@ -4496,7 +4497,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
@@ -4504,7 +4505,7 @@
         <v>132</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
@@ -4512,7 +4513,7 @@
         <v>133</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -4520,7 +4521,7 @@
         <v>134</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
@@ -4528,7 +4529,7 @@
         <v>135</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
@@ -4536,7 +4537,7 @@
         <v>136</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
@@ -4544,7 +4545,7 @@
         <v>137</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
@@ -4552,7 +4553,7 @@
         <v>138</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
@@ -4560,7 +4561,7 @@
         <v>139</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
@@ -4568,7 +4569,7 @@
         <v>140</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
@@ -4576,7 +4577,7 @@
         <v>141</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
@@ -4584,7 +4585,7 @@
         <v>142</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -4592,7 +4593,7 @@
         <v>143</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
@@ -4600,7 +4601,7 @@
         <v>144</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
@@ -4608,7 +4609,7 @@
         <v>145</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -4616,7 +4617,7 @@
         <v>146</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
@@ -4624,7 +4625,7 @@
         <v>147</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
@@ -4632,7 +4633,7 @@
         <v>148</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -4640,7 +4641,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
@@ -4648,7 +4649,7 @@
         <v>150</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
@@ -4656,7 +4657,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
@@ -4664,7 +4665,7 @@
         <v>152</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
@@ -4672,7 +4673,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
@@ -4680,7 +4681,7 @@
         <v>154</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
@@ -4688,7 +4689,7 @@
         <v>155</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
@@ -4696,7 +4697,7 @@
         <v>156</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -4704,7 +4705,7 @@
         <v>157</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
@@ -4712,7 +4713,7 @@
         <v>158</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
@@ -4720,7 +4721,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
@@ -4728,7 +4729,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
@@ -4736,7 +4737,7 @@
         <v>161</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -4744,7 +4745,7 @@
         <v>162</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
@@ -4752,7 +4753,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -4760,7 +4761,7 @@
         <v>164</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
@@ -4768,7 +4769,7 @@
         <v>165</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
@@ -4776,7 +4777,7 @@
         <v>166</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
@@ -4784,7 +4785,7 @@
         <v>167</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
@@ -4792,7 +4793,7 @@
         <v>168</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
@@ -4800,7 +4801,7 @@
         <v>169</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
@@ -4808,7 +4809,7 @@
         <v>170</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
@@ -4816,7 +4817,7 @@
         <v>171</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
@@ -4824,7 +4825,7 @@
         <v>172</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
@@ -4832,7 +4833,7 @@
         <v>173</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
@@ -4840,7 +4841,7 @@
         <v>174</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
@@ -4848,7 +4849,7 @@
         <v>175</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
@@ -4856,7 +4857,7 @@
         <v>176</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
@@ -4864,7 +4865,7 @@
         <v>177</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
@@ -4872,7 +4873,7 @@
         <v>178</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
@@ -4880,7 +4881,7 @@
         <v>179</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
@@ -4888,7 +4889,7 @@
         <v>180</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
@@ -4896,7 +4897,7 @@
         <v>181</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -4904,7 +4905,7 @@
         <v>182</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
@@ -4912,7 +4913,7 @@
         <v>183</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
@@ -4920,7 +4921,7 @@
         <v>184</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
@@ -4928,7 +4929,7 @@
         <v>185</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
@@ -4936,7 +4937,7 @@
         <v>186</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
@@ -4944,7 +4945,7 @@
         <v>187</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
@@ -4952,7 +4953,7 @@
         <v>188</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
@@ -4960,7 +4961,7 @@
         <v>189</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
@@ -4968,7 +4969,7 @@
         <v>190</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
@@ -4976,7 +4977,7 @@
         <v>191</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
@@ -4984,7 +4985,7 @@
         <v>192</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
@@ -4992,7 +4993,7 @@
         <v>193</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
@@ -5000,7 +5001,7 @@
         <v>194</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
@@ -5008,7 +5009,7 @@
         <v>195</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
@@ -5016,7 +5017,7 @@
         <v>196</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
@@ -5024,7 +5025,7 @@
         <v>197</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
@@ -5032,7 +5033,7 @@
         <v>198</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
@@ -5040,7 +5041,7 @@
         <v>199</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
@@ -5048,7 +5049,7 @@
         <v>200</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
@@ -5056,7 +5057,7 @@
         <v>201</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
@@ -5064,7 +5065,7 @@
         <v>202</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
@@ -5072,7 +5073,7 @@
         <v>203</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
@@ -5080,7 +5081,7 @@
         <v>204</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
@@ -5088,7 +5089,7 @@
         <v>205</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
@@ -5096,7 +5097,7 @@
         <v>206</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
@@ -5104,7 +5105,7 @@
         <v>207</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
@@ -5112,7 +5113,7 @@
         <v>208</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
@@ -5120,7 +5121,7 @@
         <v>209</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
@@ -5128,7 +5129,7 @@
         <v>210</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
@@ -5136,7 +5137,7 @@
         <v>211</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
@@ -5144,7 +5145,7 @@
         <v>212</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
@@ -5152,7 +5153,7 @@
         <v>213</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
@@ -5160,7 +5161,7 @@
         <v>214</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
@@ -5168,7 +5169,7 @@
         <v>215</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
@@ -5176,7 +5177,7 @@
         <v>216</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
@@ -5184,7 +5185,7 @@
         <v>217</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
@@ -5192,7 +5193,7 @@
         <v>218</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
@@ -5200,7 +5201,7 @@
         <v>219</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
@@ -5208,7 +5209,7 @@
         <v>220</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
@@ -5216,7 +5217,7 @@
         <v>221</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -5224,7 +5225,7 @@
         <v>222</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
@@ -5232,7 +5233,7 @@
         <v>223</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
@@ -5240,7 +5241,7 @@
         <v>224</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
@@ -5248,7 +5249,7 @@
         <v>225</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
@@ -5256,7 +5257,7 @@
         <v>226</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
@@ -5264,7 +5265,7 @@
         <v>227</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.35">
@@ -5272,7 +5273,7 @@
         <v>228</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.35">
@@ -5280,7 +5281,7 @@
         <v>229</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.35">
@@ -5288,7 +5289,7 @@
         <v>230</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.35">
@@ -5296,7 +5297,7 @@
         <v>231</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.35">
@@ -5304,7 +5305,7 @@
         <v>232</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.35">
@@ -5312,7 +5313,7 @@
         <v>233</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.35">
@@ -5320,7 +5321,7 @@
         <v>234</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.35">
@@ -5328,7 +5329,7 @@
         <v>235</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.35">
@@ -5336,7 +5337,7 @@
         <v>236</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.35">
@@ -5344,7 +5345,7 @@
         <v>237</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.35">
@@ -5352,7 +5353,7 @@
         <v>238</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.35">
@@ -5360,7 +5361,7 @@
         <v>239</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.35">
@@ -5368,7 +5369,7 @@
         <v>240</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.35">
@@ -5376,7 +5377,7 @@
         <v>241</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.35">
@@ -5384,7 +5385,7 @@
         <v>242</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.35">
@@ -5392,7 +5393,7 @@
         <v>243</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.35">
@@ -5400,7 +5401,7 @@
         <v>244</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.35">
@@ -5408,7 +5409,7 @@
         <v>245</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.35">
@@ -5416,7 +5417,7 @@
         <v>246</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.35">
@@ -5424,7 +5425,7 @@
         <v>247</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.35">
@@ -5432,7 +5433,7 @@
         <v>248</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.35">
@@ -5440,7 +5441,7 @@
         <v>249</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.35">
@@ -5448,7 +5449,7 @@
         <v>250</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.35">
@@ -5456,7 +5457,7 @@
         <v>251</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.35">
@@ -5464,7 +5465,7 @@
         <v>252</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.35">
@@ -5472,7 +5473,7 @@
         <v>253</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.35">
@@ -5480,7 +5481,7 @@
         <v>254</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.35">
@@ -5488,7 +5489,7 @@
         <v>255</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.35">
@@ -5496,7 +5497,7 @@
         <v>256</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.35">
@@ -5504,7 +5505,7 @@
         <v>257</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.35">
@@ -5512,7 +5513,7 @@
         <v>258</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.35">
@@ -5520,7 +5521,7 @@
         <v>259</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>761</v>
+        <v>999</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.35">
@@ -5528,7 +5529,7 @@
         <v>260</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.35">
@@ -5536,7 +5537,7 @@
         <v>261</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -5544,7 +5545,7 @@
         <v>262</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.35">
@@ -5552,7 +5553,7 @@
         <v>263</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.35">
@@ -5560,7 +5561,7 @@
         <v>264</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.35">
@@ -5568,7 +5569,7 @@
         <v>265</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.35">
@@ -5576,7 +5577,7 @@
         <v>266</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -5584,7 +5585,7 @@
         <v>267</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.35">
@@ -5592,7 +5593,7 @@
         <v>268</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.35">
@@ -5600,7 +5601,7 @@
         <v>269</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -5608,7 +5609,7 @@
         <v>270</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.35">
@@ -5616,7 +5617,7 @@
         <v>271</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.35">
@@ -5624,7 +5625,7 @@
         <v>272</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.35">
@@ -5632,7 +5633,7 @@
         <v>273</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.35">
@@ -5640,7 +5641,7 @@
         <v>274</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.35">
@@ -5648,7 +5649,7 @@
         <v>275</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.35">
@@ -5656,7 +5657,7 @@
         <v>276</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.35">
@@ -5664,7 +5665,7 @@
         <v>277</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.35">
@@ -5672,7 +5673,7 @@
         <v>278</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.35">
@@ -5680,7 +5681,7 @@
         <v>279</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.35">
@@ -5688,7 +5689,7 @@
         <v>280</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.35">
@@ -5696,7 +5697,7 @@
         <v>281</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.35">
@@ -5704,7 +5705,7 @@
         <v>282</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.35">
@@ -5712,7 +5713,7 @@
         <v>283</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.35">
@@ -5720,7 +5721,7 @@
         <v>284</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.35">
@@ -5728,7 +5729,7 @@
         <v>285</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.35">
@@ -5736,7 +5737,7 @@
         <v>286</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.35">
@@ -5744,7 +5745,7 @@
         <v>287</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.35">
@@ -5752,7 +5753,7 @@
         <v>288</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.35">
@@ -5760,7 +5761,7 @@
         <v>289</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.35">
@@ -5768,7 +5769,7 @@
         <v>290</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.35">
@@ -5776,7 +5777,7 @@
         <v>291</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.35">
@@ -5784,7 +5785,7 @@
         <v>292</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>794</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.35">
@@ -5792,7 +5793,7 @@
         <v>293</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.35">
@@ -5800,7 +5801,7 @@
         <v>294</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -5808,7 +5809,7 @@
         <v>295</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.35">
@@ -5816,7 +5817,7 @@
         <v>296</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.35">
@@ -5824,7 +5825,7 @@
         <v>297</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.35">
@@ -5832,7 +5833,7 @@
         <v>298</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.35">
@@ -5840,7 +5841,7 @@
         <v>299</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.35">
@@ -5848,7 +5849,7 @@
         <v>300</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.35">
@@ -5856,7 +5857,7 @@
         <v>301</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.35">
@@ -5864,7 +5865,7 @@
         <v>302</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.35">
@@ -5872,7 +5873,7 @@
         <v>303</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.35">
@@ -5880,7 +5881,7 @@
         <v>304</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.35">
@@ -5888,7 +5889,7 @@
         <v>305</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.35">
@@ -5896,7 +5897,7 @@
         <v>306</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.35">
@@ -5904,7 +5905,7 @@
         <v>307</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.35">
@@ -5912,7 +5913,7 @@
         <v>308</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.35">
@@ -5920,7 +5921,7 @@
         <v>309</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.35">
@@ -5928,7 +5929,7 @@
         <v>310</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.35">
@@ -5936,7 +5937,7 @@
         <v>311</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.35">
@@ -5944,7 +5945,7 @@
         <v>312</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.35">
@@ -5952,7 +5953,7 @@
         <v>313</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.35">
@@ -5960,7 +5961,7 @@
         <v>314</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.35">
@@ -5968,7 +5969,7 @@
         <v>315</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.35">
@@ -5976,7 +5977,7 @@
         <v>316</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.35">
@@ -5984,7 +5985,7 @@
         <v>317</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.35">
@@ -5992,7 +5993,7 @@
         <v>318</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.35">
@@ -6000,7 +6001,7 @@
         <v>319</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.35">
@@ -6008,7 +6009,7 @@
         <v>320</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.35">
@@ -6016,7 +6017,7 @@
         <v>321</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.35">
@@ -6024,7 +6025,7 @@
         <v>322</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.35">
@@ -6032,7 +6033,7 @@
         <v>323</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.35">
@@ -6040,7 +6041,7 @@
         <v>324</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.35">
@@ -6048,7 +6049,7 @@
         <v>325</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.35">
@@ -6056,7 +6057,7 @@
         <v>326</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.35">
@@ -6064,7 +6065,7 @@
         <v>327</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.35">
@@ -6072,7 +6073,7 @@
         <v>328</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.35">
@@ -6080,7 +6081,7 @@
         <v>329</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.35">
@@ -6088,7 +6089,7 @@
         <v>330</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>832</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.35">
@@ -6096,7 +6097,7 @@
         <v>331</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.35">
@@ -6104,7 +6105,7 @@
         <v>332</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.35">
@@ -6112,7 +6113,7 @@
         <v>333</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.35">
@@ -6120,7 +6121,7 @@
         <v>334</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.35">
@@ -6128,7 +6129,7 @@
         <v>335</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.35">
@@ -6136,7 +6137,7 @@
         <v>336</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.35">
@@ -6144,7 +6145,7 @@
         <v>337</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.35">
@@ -6152,7 +6153,7 @@
         <v>338</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.35">
@@ -6160,7 +6161,7 @@
         <v>339</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.35">
@@ -6168,7 +6169,7 @@
         <v>340</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.35">
@@ -6176,7 +6177,7 @@
         <v>341</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.35">
@@ -6184,7 +6185,7 @@
         <v>342</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.35">
@@ -6192,7 +6193,7 @@
         <v>343</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.35">
@@ -6200,7 +6201,7 @@
         <v>344</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.35">
@@ -6208,7 +6209,7 @@
         <v>345</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.35">
@@ -6216,7 +6217,7 @@
         <v>346</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.35">
@@ -6224,7 +6225,7 @@
         <v>347</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.35">
@@ -6232,7 +6233,7 @@
         <v>348</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.35">
@@ -6240,7 +6241,7 @@
         <v>349</v>
       </c>
       <c r="B351" s="2" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.35">
@@ -6248,7 +6249,7 @@
         <v>350</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.35">
@@ -6256,7 +6257,7 @@
         <v>351</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
     </row>
     <row r="354" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -6264,7 +6265,7 @@
         <v>352</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.35">
@@ -6272,7 +6273,7 @@
         <v>353</v>
       </c>
       <c r="B355" s="2" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.35">
@@ -6280,7 +6281,7 @@
         <v>354</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.35">
@@ -6288,7 +6289,7 @@
         <v>355</v>
       </c>
       <c r="B357" s="2" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.35">
@@ -6296,7 +6297,7 @@
         <v>356</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.35">
@@ -6304,7 +6305,7 @@
         <v>357</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.35">
@@ -6312,7 +6313,7 @@
         <v>358</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.35">
@@ -6320,7 +6321,7 @@
         <v>359</v>
       </c>
       <c r="B361" s="2" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.35">
@@ -6328,7 +6329,7 @@
         <v>360</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.35">
@@ -6336,7 +6337,7 @@
         <v>361</v>
       </c>
       <c r="B363" s="2" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.35">
@@ -6344,7 +6345,7 @@
         <v>362</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.35">
@@ -6352,7 +6353,7 @@
         <v>363</v>
       </c>
       <c r="B365" s="2" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.35">
@@ -6360,7 +6361,7 @@
         <v>364</v>
       </c>
       <c r="B366" s="2" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.35">
@@ -6368,7 +6369,7 @@
         <v>365</v>
       </c>
       <c r="B367" s="2" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.35">
@@ -6376,7 +6377,7 @@
         <v>366</v>
       </c>
       <c r="B368" s="2" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.35">
@@ -6384,7 +6385,7 @@
         <v>367</v>
       </c>
       <c r="B369" s="2" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.35">
@@ -6392,7 +6393,7 @@
         <v>368</v>
       </c>
       <c r="B370" s="2" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.35">
@@ -6400,7 +6401,7 @@
         <v>369</v>
       </c>
       <c r="B371" s="2" t="s">
-        <v>871</v>
+        <v>867</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.35">
@@ -6408,7 +6409,7 @@
         <v>370</v>
       </c>
       <c r="B372" s="2" t="s">
-        <v>872</v>
+        <v>868</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.35">
@@ -6416,7 +6417,7 @@
         <v>371</v>
       </c>
       <c r="B373" s="2" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.35">
@@ -6424,7 +6425,7 @@
         <v>372</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.35">
@@ -6432,7 +6433,7 @@
         <v>373</v>
       </c>
       <c r="B375" s="2" t="s">
-        <v>875</v>
+        <v>871</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.35">
@@ -6440,7 +6441,7 @@
         <v>374</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>876</v>
+        <v>872</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.35">
@@ -6448,7 +6449,7 @@
         <v>375</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.35">
@@ -6456,7 +6457,7 @@
         <v>376</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.35">
@@ -6464,7 +6465,7 @@
         <v>377</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>879</v>
+        <v>875</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.35">
@@ -6472,7 +6473,7 @@
         <v>378</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>880</v>
+        <v>876</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.35">
@@ -6480,7 +6481,7 @@
         <v>379</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.35">
@@ -6488,7 +6489,7 @@
         <v>380</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.35">
@@ -6496,7 +6497,7 @@
         <v>381</v>
       </c>
       <c r="B383" s="2" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
     </row>
     <row r="384" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -6504,7 +6505,7 @@
         <v>382</v>
       </c>
       <c r="B384" s="2" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.35">
@@ -6512,7 +6513,7 @@
         <v>383</v>
       </c>
       <c r="B385" s="2" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.35">
@@ -6520,7 +6521,7 @@
         <v>384</v>
       </c>
       <c r="B386" s="2" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.35">
@@ -6528,7 +6529,7 @@
         <v>385</v>
       </c>
       <c r="B387" s="2" t="s">
-        <v>887</v>
+        <v>883</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.35">
@@ -6536,7 +6537,7 @@
         <v>386</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>888</v>
+        <v>884</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.35">
@@ -6544,7 +6545,7 @@
         <v>387</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>889</v>
+        <v>885</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.35">
@@ -6552,7 +6553,7 @@
         <v>388</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
     </row>
     <row r="391" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -6560,7 +6561,7 @@
         <v>389</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.35">
@@ -6568,7 +6569,7 @@
         <v>390</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>892</v>
+        <v>888</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.35">
@@ -6576,7 +6577,7 @@
         <v>391</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>893</v>
+        <v>889</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.35">
@@ -6584,7 +6585,7 @@
         <v>392</v>
       </c>
       <c r="B394" s="2" t="s">
-        <v>894</v>
+        <v>890</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.35">
@@ -6592,7 +6593,7 @@
         <v>393</v>
       </c>
       <c r="B395" s="2" t="s">
-        <v>895</v>
+        <v>891</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.35">
@@ -6600,7 +6601,7 @@
         <v>394</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>896</v>
+        <v>892</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.35">
@@ -6608,7 +6609,7 @@
         <v>395</v>
       </c>
       <c r="B397" s="2" t="s">
-        <v>897</v>
+        <v>893</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.35">
@@ -6616,7 +6617,7 @@
         <v>396</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>898</v>
+        <v>894</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.35">
@@ -6624,7 +6625,7 @@
         <v>397</v>
       </c>
       <c r="B399" s="2" t="s">
-        <v>899</v>
+        <v>895</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.35">
@@ -6632,7 +6633,7 @@
         <v>398</v>
       </c>
       <c r="B400" s="2" t="s">
-        <v>900</v>
+        <v>896</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.35">
@@ -6640,7 +6641,7 @@
         <v>399</v>
       </c>
       <c r="B401" s="2" t="s">
-        <v>901</v>
+        <v>897</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.35">
@@ -6648,7 +6649,7 @@
         <v>400</v>
       </c>
       <c r="B402" s="2" t="s">
-        <v>902</v>
+        <v>898</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.35">
@@ -6656,7 +6657,7 @@
         <v>401</v>
       </c>
       <c r="B403" s="2" t="s">
-        <v>903</v>
+        <v>899</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.35">
@@ -6664,7 +6665,7 @@
         <v>402</v>
       </c>
       <c r="B404" s="2" t="s">
-        <v>904</v>
+        <v>900</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.35">
@@ -6672,7 +6673,7 @@
         <v>403</v>
       </c>
       <c r="B405" s="2" t="s">
-        <v>905</v>
+        <v>901</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.35">
@@ -6680,7 +6681,7 @@
         <v>404</v>
       </c>
       <c r="B406" s="2" t="s">
-        <v>906</v>
+        <v>902</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.35">
@@ -6688,7 +6689,7 @@
         <v>405</v>
       </c>
       <c r="B407" s="2" t="s">
-        <v>907</v>
+        <v>903</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.35">
@@ -6696,7 +6697,7 @@
         <v>406</v>
       </c>
       <c r="B408" s="2" t="s">
-        <v>908</v>
+        <v>904</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.35">
@@ -6704,7 +6705,7 @@
         <v>407</v>
       </c>
       <c r="B409" s="2" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.35">
@@ -6712,7 +6713,7 @@
         <v>408</v>
       </c>
       <c r="B410" s="2" t="s">
-        <v>910</v>
+        <v>906</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.35">
@@ -6720,7 +6721,7 @@
         <v>409</v>
       </c>
       <c r="B411" s="2" t="s">
-        <v>911</v>
+        <v>907</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.35">
@@ -6728,7 +6729,7 @@
         <v>410</v>
       </c>
       <c r="B412" s="2" t="s">
-        <v>912</v>
+        <v>908</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.35">
@@ -6736,7 +6737,7 @@
         <v>411</v>
       </c>
       <c r="B413" s="2" t="s">
-        <v>913</v>
+        <v>909</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.35">
@@ -6744,7 +6745,7 @@
         <v>412</v>
       </c>
       <c r="B414" s="2" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.35">
@@ -6752,7 +6753,7 @@
         <v>413</v>
       </c>
       <c r="B415" s="2" t="s">
-        <v>915</v>
+        <v>911</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.35">
@@ -6760,7 +6761,7 @@
         <v>414</v>
       </c>
       <c r="B416" s="2" t="s">
-        <v>916</v>
+        <v>912</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.35">
@@ -6768,7 +6769,7 @@
         <v>415</v>
       </c>
       <c r="B417" s="2" t="s">
-        <v>917</v>
+        <v>913</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.35">
@@ -6776,7 +6777,7 @@
         <v>416</v>
       </c>
       <c r="B418" s="2" t="s">
-        <v>918</v>
+        <v>914</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.35">
@@ -6784,7 +6785,7 @@
         <v>417</v>
       </c>
       <c r="B419" s="2" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.35">
@@ -6792,7 +6793,7 @@
         <v>418</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>920</v>
+        <v>916</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.35">
@@ -6800,7 +6801,7 @@
         <v>419</v>
       </c>
       <c r="B421" s="2" t="s">
-        <v>921</v>
+        <v>917</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.35">
@@ -6808,7 +6809,7 @@
         <v>420</v>
       </c>
       <c r="B422" s="2" t="s">
-        <v>922</v>
+        <v>918</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.35">
@@ -6816,7 +6817,7 @@
         <v>421</v>
       </c>
       <c r="B423" s="2" t="s">
-        <v>923</v>
+        <v>919</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.35">
@@ -6824,7 +6825,7 @@
         <v>422</v>
       </c>
       <c r="B424" s="2" t="s">
-        <v>924</v>
+        <v>920</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.35">
@@ -6832,7 +6833,7 @@
         <v>423</v>
       </c>
       <c r="B425" s="2" t="s">
-        <v>925</v>
+        <v>921</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.35">
@@ -6840,7 +6841,7 @@
         <v>424</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>926</v>
+        <v>922</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.35">
@@ -6848,7 +6849,7 @@
         <v>425</v>
       </c>
       <c r="B427" s="2" t="s">
-        <v>927</v>
+        <v>923</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.35">
@@ -6856,7 +6857,7 @@
         <v>426</v>
       </c>
       <c r="B428" s="2" t="s">
-        <v>928</v>
+        <v>924</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.35">
@@ -6864,7 +6865,7 @@
         <v>427</v>
       </c>
       <c r="B429" s="2" t="s">
-        <v>929</v>
+        <v>925</v>
       </c>
     </row>
     <row r="430" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -6872,7 +6873,7 @@
         <v>428</v>
       </c>
       <c r="B430" s="2" t="s">
-        <v>930</v>
+        <v>926</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.35">
@@ -6880,7 +6881,7 @@
         <v>429</v>
       </c>
       <c r="B431" s="2" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.35">
@@ -6888,7 +6889,7 @@
         <v>430</v>
       </c>
       <c r="B432" s="2" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.35">
@@ -6896,7 +6897,7 @@
         <v>431</v>
       </c>
       <c r="B433" s="2" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.35">
@@ -6904,7 +6905,7 @@
         <v>432</v>
       </c>
       <c r="B434" s="2" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.35">
@@ -6912,7 +6913,7 @@
         <v>433</v>
       </c>
       <c r="B435" s="2" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.35">
@@ -6920,7 +6921,7 @@
         <v>434</v>
       </c>
       <c r="B436" s="2" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.35">
@@ -6928,7 +6929,7 @@
         <v>435</v>
       </c>
       <c r="B437" s="2" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.35">
@@ -6936,7 +6937,7 @@
         <v>436</v>
       </c>
       <c r="B438" s="2" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.35">
@@ -6944,7 +6945,7 @@
         <v>437</v>
       </c>
       <c r="B439" s="2" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.35">
@@ -6952,7 +6953,7 @@
         <v>438</v>
       </c>
       <c r="B440" s="2" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.35">
@@ -6960,7 +6961,7 @@
         <v>439</v>
       </c>
       <c r="B441" s="2" t="s">
-        <v>941</v>
+        <v>937</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.35">
@@ -6968,7 +6969,7 @@
         <v>440</v>
       </c>
       <c r="B442" s="2" t="s">
-        <v>942</v>
+        <v>938</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.35">
@@ -6976,7 +6977,7 @@
         <v>441</v>
       </c>
       <c r="B443" s="2" t="s">
-        <v>943</v>
+        <v>939</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.35">
@@ -6984,7 +6985,7 @@
         <v>442</v>
       </c>
       <c r="B444" s="2" t="s">
-        <v>944</v>
+        <v>940</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.35">
@@ -6992,7 +6993,7 @@
         <v>443</v>
       </c>
       <c r="B445" s="2" t="s">
-        <v>945</v>
+        <v>941</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.35">
@@ -7000,7 +7001,7 @@
         <v>444</v>
       </c>
       <c r="B446" s="2" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.35">
@@ -7008,7 +7009,7 @@
         <v>445</v>
       </c>
       <c r="B447" s="2" t="s">
-        <v>947</v>
+        <v>943</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.35">
@@ -7016,7 +7017,7 @@
         <v>446</v>
       </c>
       <c r="B448" s="2" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.35">
@@ -7024,7 +7025,7 @@
         <v>447</v>
       </c>
       <c r="B449" s="2" t="s">
-        <v>949</v>
+        <v>945</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.35">
@@ -7032,7 +7033,7 @@
         <v>448</v>
       </c>
       <c r="B450" s="2" t="s">
-        <v>950</v>
+        <v>946</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.35">
@@ -7040,7 +7041,7 @@
         <v>449</v>
       </c>
       <c r="B451" s="2" t="s">
-        <v>951</v>
+        <v>947</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.35">
@@ -7048,7 +7049,7 @@
         <v>450</v>
       </c>
       <c r="B452" s="2" t="s">
-        <v>952</v>
+        <v>948</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.35">
@@ -7056,7 +7057,7 @@
         <v>451</v>
       </c>
       <c r="B453" s="2" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.35">
@@ -7064,7 +7065,7 @@
         <v>452</v>
       </c>
       <c r="B454" s="2" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
     </row>
     <row r="455" spans="1:2" ht="26.2" x14ac:dyDescent="0.35">
@@ -7072,7 +7073,7 @@
         <v>453</v>
       </c>
       <c r="B455" s="2" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.35">
@@ -7080,7 +7081,7 @@
         <v>454</v>
       </c>
       <c r="B456" s="2" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.35">
@@ -7088,7 +7089,7 @@
         <v>455</v>
       </c>
       <c r="B457" s="2" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.35">
@@ -7096,7 +7097,7 @@
         <v>456</v>
       </c>
       <c r="B458" s="2" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.35">
@@ -7104,7 +7105,7 @@
         <v>457</v>
       </c>
       <c r="B459" s="2" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.35">
@@ -7112,7 +7113,7 @@
         <v>458</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.35">
@@ -7120,7 +7121,7 @@
         <v>459</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.35">
@@ -7128,7 +7129,7 @@
         <v>460</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.35">
@@ -7136,7 +7137,7 @@
         <v>461</v>
       </c>
       <c r="B463" s="2" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.35">
@@ -7144,7 +7145,7 @@
         <v>462</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.35">
@@ -7152,7 +7153,7 @@
         <v>463</v>
       </c>
       <c r="B465" s="2" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.35">
@@ -7160,7 +7161,7 @@
         <v>464</v>
       </c>
       <c r="B466" s="2" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.35">
@@ -7168,7 +7169,7 @@
         <v>465</v>
       </c>
       <c r="B467" s="2" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.35">
@@ -7176,7 +7177,7 @@
         <v>466</v>
       </c>
       <c r="B468" s="2" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.35">
@@ -7184,7 +7185,7 @@
         <v>467</v>
       </c>
       <c r="B469" s="2" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.35">
@@ -7192,7 +7193,7 @@
         <v>468</v>
       </c>
       <c r="B470" s="2" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.35">
@@ -7200,7 +7201,7 @@
         <v>469</v>
       </c>
       <c r="B471" s="2" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.35">
@@ -7208,7 +7209,7 @@
         <v>470</v>
       </c>
       <c r="B472" s="2" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.35">
@@ -7216,7 +7217,7 @@
         <v>471</v>
       </c>
       <c r="B473" s="2" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.35">
@@ -7224,7 +7225,7 @@
         <v>472</v>
       </c>
       <c r="B474" s="2" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.35">
@@ -7232,7 +7233,7 @@
         <v>473</v>
       </c>
       <c r="B475" s="2" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.35">
@@ -7240,7 +7241,7 @@
         <v>474</v>
       </c>
       <c r="B476" s="2" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.35">
@@ -7248,7 +7249,7 @@
         <v>475</v>
       </c>
       <c r="B477" s="2" t="s">
-        <v>977</v>
+        <v>973</v>
       </c>
     </row>
     <row r="478" spans="1:2" x14ac:dyDescent="0.35">
@@ -7256,7 +7257,7 @@
         <v>476</v>
       </c>
       <c r="B478" s="2" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
     </row>
     <row r="479" spans="1:2" x14ac:dyDescent="0.35">
@@ -7264,7 +7265,7 @@
         <v>477</v>
       </c>
       <c r="B479" s="2" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
     </row>
     <row r="480" spans="1:2" x14ac:dyDescent="0.35">
@@ -7272,7 +7273,7 @@
         <v>478</v>
       </c>
       <c r="B480" s="2" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
     </row>
     <row r="481" spans="1:2" x14ac:dyDescent="0.35">
@@ -7280,7 +7281,7 @@
         <v>479</v>
       </c>
       <c r="B481" s="2" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
     </row>
     <row r="482" spans="1:2" x14ac:dyDescent="0.35">
@@ -7288,7 +7289,7 @@
         <v>480</v>
       </c>
       <c r="B482" s="2" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.35">
@@ -7296,7 +7297,7 @@
         <v>481</v>
       </c>
       <c r="B483" s="2" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
     </row>
     <row r="484" spans="1:2" x14ac:dyDescent="0.35">
@@ -7304,7 +7305,7 @@
         <v>482</v>
       </c>
       <c r="B484" s="2" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
     </row>
     <row r="485" spans="1:2" x14ac:dyDescent="0.35">
@@ -7312,7 +7313,7 @@
         <v>483</v>
       </c>
       <c r="B485" s="2" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.35">
@@ -7320,7 +7321,7 @@
         <v>484</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
     </row>
     <row r="487" spans="1:2" x14ac:dyDescent="0.35">
@@ -7328,7 +7329,7 @@
         <v>485</v>
       </c>
       <c r="B487" s="2" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
     </row>
     <row r="488" spans="1:2" x14ac:dyDescent="0.35">
@@ -7336,7 +7337,7 @@
         <v>486</v>
       </c>
       <c r="B488" s="2" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
     </row>
     <row r="489" spans="1:2" x14ac:dyDescent="0.35">
@@ -7344,7 +7345,7 @@
         <v>487</v>
       </c>
       <c r="B489" s="2" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
     </row>
     <row r="490" spans="1:2" x14ac:dyDescent="0.35">
@@ -7352,7 +7353,7 @@
         <v>488</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
     </row>
     <row r="491" spans="1:2" x14ac:dyDescent="0.35">
@@ -7360,7 +7361,7 @@
         <v>489</v>
       </c>
       <c r="B491" s="2" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
     </row>
     <row r="492" spans="1:2" x14ac:dyDescent="0.35">
@@ -7368,7 +7369,7 @@
         <v>490</v>
       </c>
       <c r="B492" s="2" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
     </row>
     <row r="493" spans="1:2" x14ac:dyDescent="0.35">
@@ -7376,7 +7377,7 @@
         <v>491</v>
       </c>
       <c r="B493" s="2" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
     </row>
     <row r="494" spans="1:2" x14ac:dyDescent="0.35">
@@ -7384,7 +7385,7 @@
         <v>492</v>
       </c>
       <c r="B494" s="2" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
     </row>
     <row r="495" spans="1:2" x14ac:dyDescent="0.35">
@@ -7392,7 +7393,7 @@
         <v>493</v>
       </c>
       <c r="B495" s="2" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
     </row>
     <row r="496" spans="1:2" x14ac:dyDescent="0.35">
@@ -7400,7 +7401,7 @@
         <v>494</v>
       </c>
       <c r="B496" s="2" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
     </row>
     <row r="497" spans="1:2" x14ac:dyDescent="0.35">
@@ -7408,7 +7409,7 @@
         <v>495</v>
       </c>
       <c r="B497" s="2" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
     </row>
     <row r="498" spans="1:2" x14ac:dyDescent="0.35">
@@ -7416,7 +7417,7 @@
         <v>496</v>
       </c>
       <c r="B498" s="2" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
     </row>
     <row r="499" spans="1:2" x14ac:dyDescent="0.35">
@@ -7424,7 +7425,7 @@
         <v>497</v>
       </c>
       <c r="B499" s="2" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
     </row>
     <row r="500" spans="1:2" x14ac:dyDescent="0.35">
@@ -7432,7 +7433,7 @@
         <v>498</v>
       </c>
       <c r="B500" s="2" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
     </row>
     <row r="501" spans="1:2" x14ac:dyDescent="0.35">
@@ -7440,7 +7441,7 @@
         <v>499</v>
       </c>
       <c r="B501" s="2" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
     </row>
     <row r="502" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>